<commit_message>
golden waveform for RRRR_m_s & RRRRR_m_d
</commit_message>
<xml_diff>
--- a/golden_results/waveform_result_RRRRRmiss_diff.xlsx
+++ b/golden_results/waveform_result_RRRRRmiss_diff.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\au\cacheCmodel\golden_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B7406A1-F1EC-4F3F-87E9-D3144C1D5BDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608AC742-4AF8-41D2-A2C8-F4CE6F9A7B32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8892" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8892" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="waveform_result" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1107,7 +1107,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK21"/>
   <sheetViews>
     <sheetView topLeftCell="Q1" workbookViewId="0">
@@ -3496,16 +3496,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>